<commit_message>
Update examples for improved dict handling
</commit_message>
<xml_diff>
--- a/basics/passing_dicts.xlsx
+++ b/basics/passing_dicts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13895F3-4A70-4E34-9CE9-A7DB45746A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E2C8A1-014C-436C-BF6B-79FAFFBCF7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3986" yWindow="1577" windowWidth="22208" windowHeight="13183" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -113,8 +113,8 @@
     <t>This workbook shows how to use dictionaries created in Python.
 The Python module passing_dicts.py contains various functions that operate on Python dictionaries containing the details of a person: the person's first name, last name and age.
 The Python function create_person_dict(..) creates a dictionary with keys of "first_name", "last_name" and "age". These dictionaries are automatically cached within xlSlim, the cache handles are returned in cells B9:D9
-These cache handles can then be passed to objects expecting these dictionaries. This is illustrated by the describe(..) function as shown in cells B10:D10
-More than one of the cache handles can be passed to functions as individual parameters, for example average_age(..) expect three dictionaries. This is shown in cell B11
+These cache handles can then be passed to objects expecting these dictionaries. This is illustrated by the describe_from_handle(..) function as shown in cells B10:D10
+B11 shows how a list of cache handles can be passed to the function average_age(..) which expects a list of dictionaries.
 Note how xlSlim uses Python type hinting to know which functions expect and return dictionaries. Also note how the code in passing_dicts.py was not modified to work with xlSlim.</t>
   </si>
 </sst>
@@ -300,6 +300,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4"/>
+    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -318,7 +319,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
@@ -641,7 +641,7 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -736,15 +736,15 @@
       </c>
       <c r="B9" s="3" t="str" cm="1">
         <f t="array" ref="B9">_xll.create_person_dict(B6,B7,B8)</f>
-        <v>[passing_dicts.xlsx]Sheet1$B$9@21</v>
+        <v>[passing_dicts.xlsx]Sheet1$B$9@1</v>
       </c>
       <c r="C9" s="3" t="str" cm="1">
         <f t="array" ref="C9">_xll.create_person_dict(C6,C7,C8)</f>
-        <v>[passing_dicts.xlsx]Sheet1$C$9@20</v>
+        <v>[passing_dicts.xlsx]Sheet1$C$9@1</v>
       </c>
       <c r="D9" s="3" t="str" cm="1">
         <f t="array" ref="D9">_xll.create_person_dict(D6,D7,D8)</f>
-        <v>[passing_dicts.xlsx]Sheet1$D$9@20</v>
+        <v>[passing_dicts.xlsx]Sheet1$D$9@1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
@@ -752,15 +752,15 @@
         <v>14</v>
       </c>
       <c r="B10" s="3" t="str" cm="1">
-        <f t="array" ref="B10">_xll.describe(B9)</f>
+        <f t="array" ref="B10">_xll.describe_from_handle(B9)</f>
         <v>Bob Smith is 25 years old.</v>
       </c>
       <c r="C10" s="3" t="str" cm="1">
-        <f t="array" ref="C10">_xll.describe(C9)</f>
+        <f t="array" ref="C10">_xll.describe_from_handle(C9)</f>
         <v>Alice Jones is 52 years old.</v>
       </c>
       <c r="D10" s="3" t="str" cm="1">
-        <f t="array" ref="D10">_xll.describe(D9)</f>
+        <f t="array" ref="D10">_xll.describe_from_handle(D9)</f>
         <v>John Harris is 33 years old.</v>
       </c>
     </row>
@@ -768,8 +768,8 @@
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="14" cm="1">
-        <f t="array" ref="B11">_xll.average_age(B9,C9,D9)</f>
+      <c r="B11" s="8" cm="1">
+        <f t="array" ref="B11">_xll.average_age(B9:D9)</f>
         <v>36.666666666666664</v>
       </c>
     </row>
@@ -777,146 +777,146 @@
       <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="11"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="12"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="11"/>
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="12"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="11"/>
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="12"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="11"/>
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="12"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="11"/>
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="12"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="11"/>
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="11"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="12"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="11"/>
+      <c r="A21" s="11"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="11"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A23" s="10"/>
-      <c r="B23" s="10"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="11"/>
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="11"/>
+      <c r="D23" s="11"/>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="12"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="11"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11"/>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="12"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="11"/>
+      <c r="A25" s="11"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+      <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A26" s="12"/>
-      <c r="B26" s="12"/>
-      <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="13"/>
+      <c r="A26" s="13"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -928,12 +928,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1069,15 +1066,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1101,17 +1109,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update passing dict and object examples to show direct creation of classes and dicts.
</commit_message>
<xml_diff>
--- a/basics/passing_dicts.xlsx
+++ b/basics/passing_dicts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\xlslim-code-samples\basics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45E2C8A1-014C-436C-BF6B-79FAFFBCF7F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56FA31E-CE3E-4DB0-BFB4-74275F7FB969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{257F9B7E-B69A-46EF-8C88-E8306DB661FD}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Workbook location</t>
   </si>
@@ -74,15 +74,6 @@
     <t>People</t>
   </si>
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
-    <t>Last Name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>Bob</t>
   </si>
   <si>
@@ -99,9 +90,6 @@
   </si>
   <si>
     <t>Harris</t>
-  </si>
-  <si>
-    <t>Cached Person Objects</t>
   </si>
   <si>
     <t>Descriptions</t>
@@ -116,6 +104,21 @@
 These cache handles can then be passed to objects expecting these dictionaries. This is illustrated by the describe_from_handle(..) function as shown in cells B10:D10
 B11 shows how a list of cache handles can be passed to the function average_age(..) which expects a list of dictionaries.
 Note how xlSlim uses Python type hinting to know which functions expect and return dictionaries. Also note how the code in passing_dicts.py was not modified to work with xlSlim.</t>
+  </si>
+  <si>
+    <t>Cached Person Dicts</t>
+  </si>
+  <si>
+    <t>first_name</t>
+  </si>
+  <si>
+    <t>last_name</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>Here we skip the factory function and create dictionaries directly from Excel ranges.</t>
   </si>
 </sst>
 </file>
@@ -638,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{774E7E1C-D275-4DD4-9028-FA14541EA3B8}">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -651,9 +654,10 @@
     <col min="3" max="3" width="23.3828125" customWidth="1"/>
     <col min="4" max="4" width="25.3828125" customWidth="1"/>
     <col min="5" max="5" width="25.4609375" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -663,7 +667,7 @@
       </c>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -673,7 +677,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
@@ -683,42 +687,47 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D7" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B8" s="7">
         <v>25</v>
@@ -729,8 +738,11 @@
       <c r="D8" s="7">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -747,9 +759,9 @@
         <v>[passing_dicts.xlsx]Sheet1$D$9@1</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B10" s="3" t="str" cm="1">
         <f t="array" ref="B10">_xll.describe_from_handle(B9)</f>
@@ -763,22 +775,37 @@
         <f t="array" ref="D10">_xll.describe_from_handle(D9)</f>
         <v>John Harris is 33 years old.</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="F10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="3" t="str" cm="1">
+        <f t="array" ref="G10">_xll.describe(_xll.CreateRange($A6:$A8,B6:B8))</f>
+        <v>Bob Smith is 25 years old.</v>
+      </c>
+      <c r="H10" s="3" t="str" cm="1">
+        <f t="array" ref="H10">_xll.describe(_xll.CreateRange($A6:$A8,C6:C8))</f>
+        <v>Alice Jones is 52 years old.</v>
+      </c>
+      <c r="I10" s="3" t="str" cm="1">
+        <f t="array" ref="I10">_xll.describe(_xll.CreateRange($A6:$A8,D6:D8))</f>
+        <v>John Harris is 33 years old.</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" s="8" cm="1">
         <f t="array" ref="B11">_xll.average_age(B9:D9)</f>
         <v>36.666666666666664</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" ht="14.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A13" s="9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -788,7 +815,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
       <c r="C14" s="11"/>
@@ -798,7 +825,7 @@
       <c r="G14" s="11"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
       <c r="C15" s="11"/>
@@ -808,7 +835,7 @@
       <c r="G15" s="11"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
@@ -919,8 +946,9 @@
       <c r="H26" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A13:H26"/>
+    <mergeCell ref="F7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -928,9 +956,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1066,26 +1097,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1109,9 +1129,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1FE1A4A2-BF99-4D94-B73F-D9211460B53D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B898F4E-8707-4CA2-9F8B-513D2A3B8BD6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a95c0ba0-d2e6-4b25-b7d5-a719ecc5544a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>